<commit_message>
modified the folder structure
</commit_message>
<xml_diff>
--- a/HTML.maker.xlsx
+++ b/HTML.maker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Newton\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Newton\Documents\我的坚果云\GitHub\#Report_All_in_One\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B550C95-3B03-4D1D-838B-9D81AA7D6D0B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA82F499-30B1-4D07-8DD8-27FAF915A464}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32914" windowHeight="13886" xr2:uid="{83FE33BA-6C84-4E3E-9D7F-802F5A33D210}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32918" windowHeight="13883" xr2:uid="{83FE33BA-6C84-4E3E-9D7F-802F5A33D210}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>培养类别</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,14 +107,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>计算机基础(1) + 实验</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>计算机基础(2) + 实验</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>学术训练与综合实践</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -179,11 +171,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>实验</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>论文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公共思想课</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>体育课</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算机基础</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大学英语</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -242,7 +246,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -252,11 +256,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -576,21 +583,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD7B7739-4033-4614-95EF-BC3A4F7AB7E4}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.59765625" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" customWidth="1"/>
+    <col min="3" max="3" width="14.265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -604,345 +609,369 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="5">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="6"/>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="5">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" s="6"/>
+      <c r="B11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="5">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="5">
+        <v>11</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="5">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5">
+        <v>13</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="5">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="5">
+        <v>15</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="5">
+        <v>16</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="5">
+        <v>17</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="5">
+        <v>18</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="5">
+        <v>19</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="5">
+        <v>20</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="5">
+        <v>21</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="5">
+        <v>22</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="5">
+        <v>23</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="5">
+        <v>24</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="5">
+        <v>25</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="5">
+        <v>26</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="2">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="C28" s="5">
+        <v>27</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="3">
-        <v>3</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="3">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="3">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="3">
-        <v>6</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="3">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="3">
-        <v>8</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="3">
-        <v>9</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="3">
-        <v>10</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="3">
-        <v>11</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="3">
-        <v>12</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="3">
-        <v>13</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="3">
-        <v>14</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="3">
-        <v>15</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="3">
-        <v>16</v>
-      </c>
-      <c r="D17" s="4" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="5">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="3">
-        <v>17</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="D29" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="5">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="3">
-        <v>18</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="3">
-        <v>19</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="3">
-        <v>20</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="3">
-        <v>21</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="3">
-        <v>22</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="3">
+      <c r="D30" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="3">
-        <v>24</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="3">
-        <v>25</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="3">
-        <v>26</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="3">
-        <v>27</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="A16:A25"/>
-    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="A18:A27"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" xr:uid="{681F1EFA-0717-4417-B3F6-83BC3B2170E7}"/>
-    <hyperlink ref="D19" r:id="rId2" xr:uid="{94C8E8B8-6A55-4409-A900-7B64D14436D1}"/>
-    <hyperlink ref="D20" r:id="rId3" xr:uid="{8C2F58D6-A855-4E66-8B41-8B182D83DE2A}"/>
-    <hyperlink ref="D21" r:id="rId4" xr:uid="{1E4A6FFE-F147-41CB-80D9-A920AA87A466}"/>
-    <hyperlink ref="D22" r:id="rId5" xr:uid="{8231D43D-A08F-4DBE-A5DC-B7E0CCEB27C1}"/>
-    <hyperlink ref="D23" r:id="rId6" xr:uid="{C28B5744-9D2D-4286-B49D-9BAB137398F7}"/>
-    <hyperlink ref="D24" r:id="rId7" xr:uid="{462765EA-FF30-4257-B90D-157226527454}"/>
-    <hyperlink ref="D25" r:id="rId8" xr:uid="{A58A1420-00B5-40E2-BDC0-77D65ECFCEF7}"/>
-    <hyperlink ref="D16" r:id="rId9" xr:uid="{0DF0E883-8DA5-412B-BED6-EE7EA6A2A7F8}"/>
-    <hyperlink ref="D17" r:id="rId10" xr:uid="{0F3C7DC0-39B6-4E43-B24F-F034881C6B98}"/>
-    <hyperlink ref="D26" r:id="rId11" xr:uid="{BCFB84DC-EB56-433D-BC49-085F0FAA0F51}"/>
-    <hyperlink ref="D27" r:id="rId12" xr:uid="{1D88EE09-1E2F-4821-AF29-279ECA41E653}"/>
-    <hyperlink ref="D28" r:id="rId13" xr:uid="{F31B7605-956D-4FFA-B307-FCB7D51BF0C5}"/>
-    <hyperlink ref="D10" r:id="rId14" xr:uid="{B14297EE-73DF-4625-A0FA-4A3C79157B6F}"/>
-    <hyperlink ref="D11" r:id="rId15" xr:uid="{532474ED-E3B2-45CB-B89E-C334950F0555}"/>
-    <hyperlink ref="D12" r:id="rId16" xr:uid="{22B4EA51-2D8F-4901-BAC6-A2A730679DC0}"/>
-    <hyperlink ref="D13" r:id="rId17" xr:uid="{3ABDBE61-011C-429A-8D71-F8ECF432F64B}"/>
-    <hyperlink ref="D14" r:id="rId18" xr:uid="{1E30FA73-195E-46A2-A10E-194B1F88096B}"/>
-    <hyperlink ref="D15" r:id="rId19" xr:uid="{7A7311AE-1C61-4FF0-B85B-AE01EA170128}"/>
-    <hyperlink ref="D2" r:id="rId20" xr:uid="{F6E64A5C-CCEF-4655-A9A9-21671AB695BC}"/>
-    <hyperlink ref="D3" r:id="rId21" xr:uid="{BF05F590-342D-496A-8BA8-A9BE4DDE49DD}"/>
-    <hyperlink ref="D18" r:id="rId22" xr:uid="{BFCE5C04-C37E-4A62-A486-2F44508A1B24}"/>
-    <hyperlink ref="D4" r:id="rId23" xr:uid="{343C5891-0471-4BC7-85E2-E6A50E629ED3}"/>
-    <hyperlink ref="D5" r:id="rId24" xr:uid="{2C48DA25-BA9F-4DD3-B49F-48A83C4C206B}"/>
-    <hyperlink ref="D6" r:id="rId25" xr:uid="{06FA526D-7828-4E3D-902A-62E786312596}"/>
-    <hyperlink ref="D7" r:id="rId26" xr:uid="{C4102F7E-1C5A-4EA5-A797-B7C837F2AF69}"/>
-    <hyperlink ref="D8" r:id="rId27" xr:uid="{690B17B9-B867-4494-9FFB-C778E7F12F65}"/>
+    <hyperlink ref="D11" r:id="rId1" xr:uid="{EEBC815D-BD5E-49A9-9E20-11440FA54930}"/>
+    <hyperlink ref="D21" r:id="rId2" xr:uid="{30BB4653-6A5E-4346-8599-CEFD5EE391BF}"/>
+    <hyperlink ref="D22" r:id="rId3" xr:uid="{42FB8B7F-7F41-4122-881D-EA4045752EEC}"/>
+    <hyperlink ref="D23" r:id="rId4" xr:uid="{93062A63-DE27-46F1-9770-4A6F07AC15B3}"/>
+    <hyperlink ref="D24" r:id="rId5" xr:uid="{1859C1D5-0C8B-4B45-9756-9015E8DFFDCA}"/>
+    <hyperlink ref="D25" r:id="rId6" xr:uid="{79FC6580-E377-4477-A26D-17463F23FDBB}"/>
+    <hyperlink ref="D26" r:id="rId7" xr:uid="{74656334-056F-4011-80DE-3BA12EFE64D3}"/>
+    <hyperlink ref="D27" r:id="rId8" xr:uid="{2EFD6668-0A74-4CE6-971E-4115257AFAFE}"/>
+    <hyperlink ref="D18" r:id="rId9" xr:uid="{A15577AC-2A0F-4505-AC97-71FD2B765DBC}"/>
+    <hyperlink ref="D19" r:id="rId10" xr:uid="{3DAE0491-2D53-4086-83C1-62AFD94F2D60}"/>
+    <hyperlink ref="D28" r:id="rId11" xr:uid="{56F2206E-3243-4BB7-AEFA-FD8716278BDF}"/>
+    <hyperlink ref="D29" r:id="rId12" xr:uid="{CADCA8F9-B626-4C6E-A7C1-0AF1BD06FA70}"/>
+    <hyperlink ref="D30" r:id="rId13" xr:uid="{74DE0C78-A911-4D23-A0C8-756926153966}"/>
+    <hyperlink ref="D12" r:id="rId14" xr:uid="{8E9104AE-5E00-4730-9378-CECEF4D685A9}"/>
+    <hyperlink ref="D13" r:id="rId15" xr:uid="{B68DEF4D-A9EE-4713-8603-E22BED9258CD}"/>
+    <hyperlink ref="D14" r:id="rId16" xr:uid="{FCB4EB9C-47BD-44AA-9356-2B263FDD3DD7}"/>
+    <hyperlink ref="D15" r:id="rId17" xr:uid="{E867DD40-DFE2-4898-87F6-D07B2E91DA4C}"/>
+    <hyperlink ref="D16" r:id="rId18" xr:uid="{AEAA6055-92CA-46E3-AC8A-675ACE90D54A}"/>
+    <hyperlink ref="D17" r:id="rId19" xr:uid="{AF0BB368-DD19-4803-BB36-3D5B320EB9DD}"/>
+    <hyperlink ref="D5" r:id="rId20" display="计算机基础(1) + 实验" xr:uid="{3AF3E450-8228-4FF3-9635-E4BAB5346AC6}"/>
+    <hyperlink ref="D20" r:id="rId21" xr:uid="{126FC78D-2744-4769-A940-3C1B6631FB4F}"/>
+    <hyperlink ref="D6" r:id="rId22" xr:uid="{62F99C8A-87BC-4D29-A52F-A3E4F5138173}"/>
+    <hyperlink ref="D7" r:id="rId23" xr:uid="{09173E52-9484-4AA6-BAE3-D713771E57E8}"/>
+    <hyperlink ref="D8" r:id="rId24" xr:uid="{E4EF769D-6D10-48EB-9FF8-FF2801BB430E}"/>
+    <hyperlink ref="D9" r:id="rId25" xr:uid="{4FEFE1A4-FDBD-4E2F-BF6E-9B88330551BF}"/>
+    <hyperlink ref="D10" r:id="rId26" xr:uid="{530B691D-26D0-4F4E-A7F5-7E89076E075F}"/>
+    <hyperlink ref="D2" r:id="rId27" xr:uid="{D174ADF1-E9D1-4F39-A0E2-048C0AEB67C2}"/>
+    <hyperlink ref="D4" r:id="rId28" xr:uid="{FBB864CD-F164-4FEE-A797-1F789CF66E36}"/>
+    <hyperlink ref="D3" r:id="rId29" xr:uid="{649E193B-6D71-4BAC-A341-67D300206A83}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>